<commit_message>
Fixing warnings in frontend to allow for deployment
</commit_message>
<xml_diff>
--- a/backend/app/data/pantry_ingredients.xlsx
+++ b/backend/app/data/pantry_ingredients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\OneDrive\RecipeTec\recipe-finder-demo\backend\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716A3C25-FE6C-41A6-A9BA-7EF305948407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1C62F4-A113-46D3-8452-8C6578C2F672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Result 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ingredient_name</t>
   </si>
@@ -28,28 +28,16 @@
     <t>ingredient_id</t>
   </si>
   <si>
-    <t>garlic cloves</t>
-  </si>
-  <si>
     <t>olive oil</t>
   </si>
   <si>
-    <t>butter</t>
-  </si>
-  <si>
     <t>salt</t>
-  </si>
-  <si>
-    <t>onions</t>
   </si>
   <si>
     <t>vegetable oil</t>
   </si>
   <si>
     <t>water</t>
-  </si>
-  <si>
-    <t>red onions</t>
   </si>
 </sst>
 </file>
@@ -910,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -935,7 +923,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1091</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -943,7 +931,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1726</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -951,7 +939,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>318</v>
+        <v>2695</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -959,39 +947,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>2256</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>1739</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>2695</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
         <v>2739</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>2130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>